<commit_message>
rides img and name
</commit_message>
<xml_diff>
--- a/data/stalls.xlsx
+++ b/data/stalls.xlsx
@@ -11,45 +11,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Hot Dogs</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Bench</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>Bathroom</t>
-  </si>
-  <si>
-    <t>B</t>
+    <t>Panini</t>
+  </si>
+  <si>
+    <t>Tacos</t>
   </si>
   <si>
     <t>Pizza</t>
   </si>
   <si>
     <t>Ice Cream</t>
+  </si>
+  <si>
+    <t>Bubble Tea</t>
+  </si>
+  <si>
+    <t>Fried Chips</t>
+  </si>
+  <si>
+    <t>Piadina</t>
+  </si>
+  <si>
+    <t>Sweets</t>
+  </si>
+  <si>
+    <t>Cookies</t>
   </si>
 </sst>
 </file>
@@ -329,99 +326,94 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>50.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>350.0</v>
-      </c>
-      <c r="D2" s="3">
         <v>5.0</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>350.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>5.0</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>150.0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>350.0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>10</v>
-      </c>
+        <v>4.0</v>
+      </c>
+      <c r="E4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>200.0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>350.0</v>
-      </c>
-      <c r="D5" s="4">
         <v>10.0</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="E5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>250.0</v>
-      </c>
-      <c r="C6" s="4">
-        <v>350.0</v>
-      </c>
-      <c r="D6" s="4">
         <v>3.0</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>6</v>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4">
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>